<commit_message>
form output class extended
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiksimgen/Documents/Development/Python/quotation_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA018E-D743-824D-A336-1B414075DCA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1762FE7-FD93-A840-8848-48EC142D1578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="25720" windowHeight="17440" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,6 +561,9 @@
       <c r="A12">
         <v>80001003</v>
       </c>
+      <c r="B12">
+        <v>900</v>
+      </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -586,7 +589,7 @@
         <v>80001006</v>
       </c>
       <c r="B15">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C15" s="4"/>
     </row>

</xml_diff>

<commit_message>
method to fill material list in form created
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiksimgen/Documents/Development/Python/quotation_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2A751-8437-CC4E-9753-3003F1ED73ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A6D349-E913-EE43-AFA6-B7B0B5A625DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="25720" windowHeight="17440" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,9 +558,6 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>80001003</v>
-      </c>
       <c r="B12">
         <v>900</v>
       </c>
@@ -587,9 +584,6 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>80001006</v>
-      </c>
-      <c r="B15">
-        <v>1000</v>
       </c>
       <c r="C15" s="4"/>
     </row>

</xml_diff>

<commit_message>
added exception handling for when plantcode is not found in locations.json
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiksimgen/Documents/Development/Python/quotation_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A6D349-E913-EE43-AFA6-B7B0B5A625DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C693BE8-2B93-8448-B85A-19BABDE797EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="25720" windowHeight="17440" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>Quantity in IT</t>
   </si>
   <si>
-    <t>A999</t>
-  </si>
-  <si>
     <t>planner@company.com / 0049 1111 999</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Planner 19</t>
+  </si>
+  <si>
+    <t>A001</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="4"/>
     </row>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -509,10 +509,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -521,7 +521,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4"/>
     </row>

</xml_diff>

<commit_message>
connected location database with from output
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiksimgen/Documents/Development/Python/quotation_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C693BE8-2B93-8448-B85A-19BABDE797EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2790D83-BC2C-B346-A708-08A4E5436961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="25720" windowHeight="17440" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
+    <workbookView xWindow="-26680" yWindow="6280" windowWidth="11520" windowHeight="17000" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,6 +558,9 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>999</v>
+      </c>
       <c r="B12">
         <v>900</v>
       </c>
@@ -584,6 +587,9 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>80001006</v>
+      </c>
+      <c r="B15">
+        <v>9999999</v>
       </c>
       <c r="C15" s="4"/>
     </row>

</xml_diff>

<commit_message>
fixed bug where numerical plantcodes would be read as integer, resulting in type error
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiksimgen/Documents/Development/Python/quotation_tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2790D83-BC2C-B346-A708-08A4E5436961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB08089-6E30-46BF-ABC6-82F112DF6F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26680" yWindow="6280" windowWidth="11520" windowHeight="17000" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
+    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12360" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Requester Name</t>
   </si>
@@ -70,16 +69,10 @@
     <t>planner@company.com / 0049 1111 999</t>
   </si>
   <si>
-    <t>Z999</t>
-  </si>
-  <si>
     <t>Shipper Plantcode</t>
   </si>
   <si>
     <t>Planner 19</t>
-  </si>
-  <si>
-    <t>A001</t>
   </si>
 </sst>
 </file>
@@ -453,25 +446,25 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -480,7 +473,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -489,7 +482,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -498,7 +491,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -507,30 +500,30 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4552</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7">
+        <v>5740</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -539,7 +532,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>80001001</v>
       </c>
@@ -548,7 +541,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>80001002</v>
       </c>
@@ -557,7 +550,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>999</v>
       </c>
@@ -566,7 +559,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>80001004</v>
       </c>
@@ -575,7 +568,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>80001005</v>
       </c>
@@ -584,7 +577,7 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>80001006</v>
       </c>
@@ -593,27 +586,27 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -643,14 +636,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Material class extended with logic, connected to output
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB08089-6E30-46BF-ABC6-82F112DF6F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E548E46-741A-47B0-929D-33734F175ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12360" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -514,7 +514,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5740</v>
+        <v>4773</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -534,55 +534,55 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>80001001</v>
+        <v>81730878</v>
       </c>
       <c r="B10">
-        <v>500</v>
+        <v>1998</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>80001002</v>
+        <v>81731105</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>1080</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>999</v>
+        <v>81739020</v>
       </c>
       <c r="B12">
-        <v>900</v>
+        <v>513</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>80001004</v>
+        <v>81731107</v>
       </c>
       <c r="B13">
-        <v>1200</v>
+        <v>612</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>80001005</v>
+        <v>81731111</v>
       </c>
       <c r="B14">
-        <v>500</v>
+        <v>513</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>80001006</v>
+        <v>81730877</v>
       </c>
       <c r="B15">
-        <v>9999999</v>
+        <v>400</v>
       </c>
       <c r="C15" s="4"/>
     </row>
@@ -630,6 +630,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB93645-2164-5C4C-91D6-97A540730726}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Final Stable Release 1.0.0
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E548E46-741A-47B0-929D-33734F175ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C30B7C3-D428-4CDA-8D12-9C59E6F32489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4"/>
     </row>

</xml_diff>

<commit_message>
version 1.0.1: fixed bug where P2 data is not visible on first screen of logistical data tabele in APO
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C30B7C3-D428-4CDA-8D12-9C59E6F32489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD88824F-1F8C-4121-B10D-5F21439A64FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
+    <workbookView xWindow="29340" yWindow="-12372" windowWidth="22836" windowHeight="11760" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Requester Name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Planner 19</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>Z001</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -504,8 +510,8 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>4552</v>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -513,8 +519,8 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>4773</v>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -534,55 +540,55 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>81730878</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>1998</v>
+        <v>555</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>81731105</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>1080</v>
+        <v>555</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>81739020</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>513</v>
+        <v>555</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>81731107</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>612</v>
+        <v>555</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>81731111</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>513</v>
+        <v>555</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>81730877</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>400</v>
+        <v>555</v>
       </c>
       <c r="C15" s="4"/>
     </row>
@@ -613,6 +619,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
version 1.0.2: ensures app does not close before displaying error message to user
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD88824F-1F8C-4121-B10D-5F21439A64FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79778AB-90D8-4A8C-A18A-C5AA76287672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="-12372" windowWidth="22836" windowHeight="11760" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
+    <workbookView xWindow="22932" yWindow="-15396" windowWidth="33132" windowHeight="18132" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Requester Name</t>
   </si>
@@ -75,10 +75,7 @@
     <t>Planner 19</t>
   </si>
   <si>
-    <t>A001</t>
-  </si>
-  <si>
-    <t>Z001</t>
+    <t>Z999</t>
   </si>
 </sst>
 </file>
@@ -452,7 +449,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -510,8 +507,8 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
+      <c r="B6">
+        <v>4552</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -520,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -540,7 +537,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1</v>
+        <v>81730877</v>
       </c>
       <c r="B10">
         <v>555</v>
@@ -549,7 +546,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>81730878</v>
       </c>
       <c r="B11">
         <v>555</v>
@@ -557,39 +554,15 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>555</v>
-      </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>555</v>
-      </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>555</v>
-      </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>555</v>
-      </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
version 1.0.3: fixed bug introduced with v1.0.1 in logistical data extraction
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simgen.d\OneDrive - Procter and Gamble\Documents\01 SIP Appliances\Scripts\Python\Projects\quotation_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79778AB-90D8-4A8C-A18A-C5AA76287672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66779CB-C049-4E95-9435-0DA2BC33C863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-15396" windowWidth="33132" windowHeight="18132" xr2:uid="{5EF29178-B415-4746-942A-31D534F91EF0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Requester Name</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Planner 19</t>
-  </si>
-  <si>
-    <t>Z999</t>
   </si>
 </sst>
 </file>
@@ -449,7 +446,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -507,17 +504,11 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>4552</v>
-      </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -536,21 +527,9 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>81730877</v>
-      </c>
-      <c r="B10">
-        <v>555</v>
-      </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>81730878</v>
-      </c>
-      <c r="B11">
-        <v>555</v>
-      </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>